<commit_message>
WIP find specific route
</commit_message>
<xml_diff>
--- a/prisma/fkrlTgl13Juli2022.xlsx
+++ b/prisma/fkrlTgl13Juli2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5633" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5632" uniqueCount="1237">
   <si>
     <t>noka</t>
   </si>
@@ -3581,9 +3581,6 @@
   </si>
   <si>
     <t>23.50.00</t>
-  </si>
-  <si>
-    <t>23.56.00</t>
   </si>
   <si>
     <t>1900-1-1 0.00.00</t>
@@ -5268,7 +5265,7 @@
   <dimension ref="A1:AD236"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
@@ -23754,32 +23751,32 @@
       <c r="T221" s="33" t="s">
         <v>1188</v>
       </c>
-      <c r="U221" s="8" t="s">
+      <c r="U221" s="8">
+        <v>4235</v>
+      </c>
+      <c r="V221" s="33" t="s">
         <v>1189</v>
       </c>
-      <c r="V221" s="33" t="s">
+      <c r="W221" s="33" t="s">
         <v>1190</v>
-      </c>
-      <c r="W221" s="33" t="s">
-        <v>1191</v>
       </c>
       <c r="X221" s="5" t="s">
         <v>46</v>
       </c>
       <c r="Y221" s="33" t="s">
+        <v>1191</v>
+      </c>
+      <c r="Z221" s="33" t="s">
         <v>1192</v>
       </c>
-      <c r="Z221" s="33" t="s">
+      <c r="AA221" s="33" t="s">
         <v>1193</v>
       </c>
-      <c r="AA221" s="33" t="s">
+      <c r="AB221" s="33" t="s">
         <v>1194</v>
       </c>
-      <c r="AB221" s="33" t="s">
+      <c r="AC221" s="87" t="s">
         <v>1195</v>
-      </c>
-      <c r="AC221" s="87" t="s">
-        <v>1196</v>
       </c>
       <c r="AD221" s="47"/>
     </row>
@@ -23831,7 +23828,7 @@
     </row>
     <row r="223" spans="1:30">
       <c r="A223" s="13" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B223" s="14" t="s">
         <v>1081</v>
@@ -23845,7 +23842,7 @@
         <v>1146</v>
       </c>
       <c r="G223" s="30" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="H223" s="30" t="s">
         <v>1160</v>
@@ -23854,40 +23851,40 @@
         <v>1162</v>
       </c>
       <c r="J223" s="30" t="s">
+        <v>1198</v>
+      </c>
+      <c r="K223" s="35" t="s">
         <v>1199</v>
-      </c>
-      <c r="K223" s="35" t="s">
-        <v>1200</v>
       </c>
       <c r="L223" s="30" t="s">
         <v>1184</v>
       </c>
       <c r="M223" s="35" t="s">
+        <v>1200</v>
+      </c>
+      <c r="N223" s="35" t="s">
         <v>1201</v>
       </c>
-      <c r="N223" s="35" t="s">
+      <c r="O223" s="35" t="s">
         <v>1202</v>
       </c>
-      <c r="O223" s="35" t="s">
+      <c r="P223" s="30" t="s">
         <v>1203</v>
       </c>
-      <c r="P223" s="30" t="s">
+      <c r="Q223" s="35" t="s">
         <v>1204</v>
       </c>
-      <c r="Q223" s="35" t="s">
+      <c r="R223" s="35" t="s">
         <v>1205</v>
       </c>
-      <c r="R223" s="35" t="s">
+      <c r="S223" s="35" t="s">
         <v>1206</v>
       </c>
-      <c r="S223" s="35" t="s">
+      <c r="T223" s="35" t="s">
         <v>1207</v>
       </c>
-      <c r="T223" s="35" t="s">
+      <c r="U223" s="86" t="s">
         <v>1208</v>
-      </c>
-      <c r="U223" s="86" t="s">
-        <v>1209</v>
       </c>
       <c r="V223" s="33"/>
       <c r="W223" s="33"/>
@@ -23958,7 +23955,7 @@
         <v>1177</v>
       </c>
       <c r="F225" s="5" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="G225" s="5" t="s">
         <v>1159</v>
@@ -23967,7 +23964,7 @@
         <v>1162</v>
       </c>
       <c r="I225" s="80" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="J225" s="5"/>
       <c r="K225" s="33"/>
@@ -24061,7 +24058,7 @@
         <v>1169</v>
       </c>
       <c r="I227" s="80" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J227" s="5"/>
       <c r="K227" s="33"/>
@@ -24098,16 +24095,16 @@
         <v>1173</v>
       </c>
       <c r="F228" s="5" t="s">
+        <v>1210</v>
+      </c>
+      <c r="G228" s="5" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H228" s="5" t="s">
+        <v>1200</v>
+      </c>
+      <c r="I228" s="80" t="s">
         <v>1211</v>
-      </c>
-      <c r="G228" s="5" t="s">
-        <v>1210</v>
-      </c>
-      <c r="H228" s="5" t="s">
-        <v>1201</v>
-      </c>
-      <c r="I228" s="80" t="s">
-        <v>1212</v>
       </c>
       <c r="J228" s="5"/>
       <c r="K228" s="33"/>
@@ -24152,10 +24149,10 @@
         <v>1185</v>
       </c>
       <c r="H229" s="5" t="s">
+        <v>1212</v>
+      </c>
+      <c r="I229" s="80" t="s">
         <v>1213</v>
-      </c>
-      <c r="I229" s="80" t="s">
-        <v>1214</v>
       </c>
       <c r="J229" s="5"/>
       <c r="K229" s="33"/>
@@ -24195,13 +24192,13 @@
         <v>1185</v>
       </c>
       <c r="G230" s="5" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="H230" s="5" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="I230" s="80" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="J230" s="5"/>
       <c r="K230" s="33"/>
@@ -24235,19 +24232,19 @@
       <c r="C231" s="8"/>
       <c r="D231" s="5"/>
       <c r="E231" s="8" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="F231" s="5" t="s">
+        <v>1215</v>
+      </c>
+      <c r="G231" s="5" t="s">
+        <v>1213</v>
+      </c>
+      <c r="H231" s="5" t="s">
         <v>1216</v>
       </c>
-      <c r="G231" s="5" t="s">
-        <v>1214</v>
-      </c>
-      <c r="H231" s="5" t="s">
+      <c r="I231" s="80" t="s">
         <v>1217</v>
-      </c>
-      <c r="I231" s="80" t="s">
-        <v>1218</v>
       </c>
       <c r="J231" s="5"/>
       <c r="K231" s="33"/>
@@ -24284,16 +24281,16 @@
         <v>1187</v>
       </c>
       <c r="F232" s="30" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="G232" s="30" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="H232" s="30" t="s">
+        <v>1218</v>
+      </c>
+      <c r="I232" s="82" t="s">
         <v>1219</v>
-      </c>
-      <c r="I232" s="82" t="s">
-        <v>1220</v>
       </c>
       <c r="J232" s="5"/>
       <c r="K232" s="33"/>
@@ -24329,19 +24326,19 @@
       <c r="C233" s="8"/>
       <c r="D233" s="5"/>
       <c r="E233" s="8" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="F233" s="5" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G233" s="5" t="s">
         <v>1221</v>
       </c>
-      <c r="G233" s="5" t="s">
+      <c r="H233" s="5" t="s">
         <v>1222</v>
       </c>
-      <c r="H233" s="5" t="s">
+      <c r="I233" s="80" t="s">
         <v>1223</v>
-      </c>
-      <c r="I233" s="80" t="s">
-        <v>1224</v>
       </c>
       <c r="J233" s="5"/>
       <c r="K233" s="33"/>
@@ -24375,19 +24372,19 @@
       <c r="C234" s="8"/>
       <c r="D234" s="5"/>
       <c r="E234" s="31" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F234" s="32" t="s">
         <v>1225</v>
       </c>
-      <c r="F234" s="32" t="s">
+      <c r="G234" s="32" t="s">
         <v>1226</v>
       </c>
-      <c r="G234" s="32" t="s">
+      <c r="H234" s="32" t="s">
         <v>1227</v>
       </c>
-      <c r="H234" s="32" t="s">
+      <c r="I234" s="37" t="s">
         <v>1228</v>
-      </c>
-      <c r="I234" s="37" t="s">
-        <v>1229</v>
       </c>
       <c r="J234" s="5"/>
       <c r="K234" s="33"/>
@@ -24421,19 +24418,19 @@
       <c r="C235" s="8"/>
       <c r="D235" s="5"/>
       <c r="E235" s="8" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="G235" s="5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="H235" s="5" t="s">
         <v>1230</v>
       </c>
-      <c r="H235" s="5" t="s">
+      <c r="I235" s="80" t="s">
         <v>1231</v>
-      </c>
-      <c r="I235" s="80" t="s">
-        <v>1232</v>
       </c>
       <c r="J235" s="5"/>
       <c r="K235" s="33"/>
@@ -24467,19 +24464,19 @@
       <c r="C236" s="77"/>
       <c r="D236" s="78"/>
       <c r="E236" s="77" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F236" s="78" t="s">
         <v>1233</v>
       </c>
-      <c r="F236" s="78" t="s">
+      <c r="G236" s="78" t="s">
         <v>1234</v>
       </c>
-      <c r="G236" s="78" t="s">
+      <c r="H236" s="78" t="s">
         <v>1235</v>
       </c>
-      <c r="H236" s="78" t="s">
+      <c r="I236" s="84" t="s">
         <v>1236</v>
-      </c>
-      <c r="I236" s="84" t="s">
-        <v>1237</v>
       </c>
       <c r="J236" s="78"/>
       <c r="K236" s="85"/>

</xml_diff>